<commit_message>
Termino readme, añado mejoras, incluyo más frases, añado jupyter con ejemplo subiendo mensajes en lote desde execl con pandas
</commit_message>
<xml_diff>
--- a/input/frases2.xlsx
+++ b/input/frases2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soyungalgo/Documents/GitHub/Project.4-Creating_an_API/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623C31A5-344B-7C44-95DC-F39C50C427EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F9DD1B-0D47-5D4A-A9EB-E74341894661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14440" xr2:uid="{0F49D5F3-F527-4C48-8865-7DCFA442ACE4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Once</t>
   </si>
@@ -130,6 +130,66 @@
   </si>
   <si>
     <t>¿donde está tu hermano?¿No ha venido a dormir?</t>
+  </si>
+  <si>
+    <t>No puedes aceptar trabajos si yo tengo turno de noche, alguien tiene que encargarse de Will.</t>
+  </si>
+  <si>
+    <t>family_byers</t>
+  </si>
+  <si>
+    <t>Tranquila, no te preocupes, seguro que se habrá ido temprano al colegio.</t>
+  </si>
+  <si>
+    <t>Tiene un par de amigos, pero la mayoría se ríen de el, de su ropa. Es un chico sensible, no es como los demás.</t>
+  </si>
+  <si>
+    <t>Encuentra a mi hijo. </t>
+  </si>
+  <si>
+    <t>Karen Wheeler</t>
+  </si>
+  <si>
+    <t>Mañana hay cole, acabo de acostar a Holly, Terminad el fin de semana.</t>
+  </si>
+  <si>
+    <t>Le gusto, pero no de esa forma. Nos enrollamos un par de veces.</t>
+  </si>
+  <si>
+    <t>Nancy Wheeler</t>
+  </si>
+  <si>
+    <t>No puedo, tengo que estudiar, esos exámenes son imposibles.</t>
+  </si>
+  <si>
+    <t>Jim Hopper</t>
+  </si>
+  <si>
+    <t>Estoy más guapo que tu mujer está mañana cuando la he dejado</t>
+  </si>
+  <si>
+    <t>Dr. Owens</t>
+  </si>
+  <si>
+    <t>Hemos cerrado esta zona siguiendo el protocolo de cuarentena</t>
+  </si>
+  <si>
+    <t>Me meteré en tu cabeza siempre que quiera</t>
+  </si>
+  <si>
+    <t>Kali</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Tu hermana ya era imbécil antes</t>
+  </si>
+  <si>
+    <t>Lánzale una bola de fuego</t>
+  </si>
+  <si>
+    <t>Es como esar en casa, pero es tan oscuro… es tan oscuro y vacío…</t>
   </si>
 </sst>
 </file>
@@ -512,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB298A1-276B-4548-B48E-EC62EC894699}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +797,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>32</v>
@@ -748,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>33</v>
@@ -759,63 +819,154 @@
         <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="2"/>
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="2"/>
+      <c r="A28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="2"/>
+      <c r="A31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
@@ -922,47 +1073,31 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
-      <c r="B60" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B60" s="1"/>
       <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
-      <c r="B61" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B61" s="1"/>
       <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B62" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B62" s="1"/>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B63" s="1"/>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>1</v>
-      </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B65" s="1"/>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
-      <c r="B66" t="s">
-        <v>1</v>
-      </c>
       <c r="C66" s="2"/>
     </row>
   </sheetData>

</xml_diff>